<commit_message>
fixing scenario add customer
</commit_message>
<xml_diff>
--- a/Data Files/LOS_Customer_TestData.xlsx
+++ b/Data Files/LOS_Customer_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\automation-taf-project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FC6042-8098-4BA4-823E-1943EBB4313B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB667E-5B96-42D9-82AD-C086B3877C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{BB2015A2-793C-446E-A619-E1E11BD5D040}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{BB2015A2-793C-446E-A619-E1E11BD5D040}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="383">
   <si>
     <t>Username</t>
   </si>
@@ -761,9 +761,6 @@
     <t>FAIE</t>
   </si>
   <si>
-    <t>1 = isInternalEmployee</t>
-  </si>
-  <si>
     <t>DEWU</t>
   </si>
   <si>
@@ -1182,6 +1179,9 @@
   </si>
   <si>
     <t>3604283107950093</t>
+  </si>
+  <si>
+    <t>Y/N</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1585,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1707,14 +1707,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BA1AD0-7BFC-40B0-8219-A5C3FF6E1E54}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.453125" customWidth="1"/>
     <col min="6" max="6" width="12.90625" bestFit="1" customWidth="1"/>
@@ -1767,13 +1768,13 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>54</v>
@@ -1788,10 +1789,10 @@
         <v>53</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1908,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF85E20-BF5A-491B-8BD8-8C65920F3112}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1929,7 +1930,8 @@
     <col min="13" max="13" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.453125" customWidth="1"/>
     <col min="15" max="15" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.453125" customWidth="1"/>
+    <col min="17" max="17" width="9.6328125" customWidth="1"/>
     <col min="18" max="18" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.90625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23.6328125" bestFit="1" customWidth="1"/>
@@ -2146,6 +2148,12 @@
       <c r="P8" t="s">
         <v>140</v>
       </c>
+      <c r="Q8" t="s">
+        <v>382</v>
+      </c>
+      <c r="T8" t="s">
+        <v>382</v>
+      </c>
       <c r="V8" t="s">
         <v>140</v>
       </c>
@@ -2157,10 +2165,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78014918-227A-4AF6-B3BB-0B6F0E9D6C98}">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2991,6 +2999,11 @@
       </c>
       <c r="U13" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -3220,8 +3233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE94967-9968-4388-93D5-8EE5D91AC311}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3284,10 +3297,10 @@
         <v>163</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>345</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>164</v>
@@ -3296,25 +3309,25 @@
         <v>165</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>340</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>341</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>166</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>245</v>
-      </c>
       <c r="U1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
@@ -3337,7 +3350,7 @@
         <v>170</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="H2" t="s">
         <v>167</v>
@@ -3358,7 +3371,7 @@
         <v>189</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>146</v>
+        <v>377</v>
       </c>
       <c r="O2" t="s">
         <v>174</v>
@@ -3393,7 +3406,7 @@
         <v>177</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="H3" t="s">
         <v>167</v>
@@ -3414,7 +3427,7 @@
         <v>193</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>15</v>
+        <v>376</v>
       </c>
       <c r="O3" t="s">
         <v>174</v>
@@ -3449,7 +3462,7 @@
         <v>181</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="H4" t="s">
         <v>167</v>
@@ -3470,7 +3483,7 @@
         <v>194</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>146</v>
+        <v>377</v>
       </c>
       <c r="O4" t="s">
         <v>174</v>
@@ -3505,7 +3518,7 @@
         <v>186</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
       <c r="H5" t="s">
         <v>167</v>
@@ -3526,7 +3539,7 @@
         <v>195</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>15</v>
+        <v>376</v>
       </c>
       <c r="O5" t="s">
         <v>174</v>
@@ -3543,13 +3556,11 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G7" t="s">
-        <v>242</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="Q9" s="4" t="s">
-        <v>341</v>
-      </c>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="Q10" s="9"/>
@@ -3564,7 +3575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4BC9DE-FDC7-4630-99DC-CABF00157D5F}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -3585,19 +3596,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>251</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>81</v>
@@ -3641,25 +3652,25 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" t="s">
         <v>252</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" t="s">
         <v>256</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I2" t="s">
-        <v>257</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>16</v>
@@ -3668,7 +3679,7 @@
         <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M2" t="s">
         <v>117</v>
@@ -3694,25 +3705,25 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" t="s">
         <v>258</v>
       </c>
-      <c r="C3" t="s">
-        <v>259</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I3" t="s">
         <v>256</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" t="s">
-        <v>257</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>142</v>
@@ -3721,7 +3732,7 @@
         <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M3" t="s">
         <v>125</v>
@@ -3747,25 +3758,25 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" t="s">
         <v>260</v>
       </c>
-      <c r="C4" t="s">
-        <v>261</v>
-      </c>
       <c r="D4" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I4" t="s">
         <v>256</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I4" t="s">
-        <v>257</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>143</v>
@@ -3774,7 +3785,7 @@
         <v>144</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M4" t="s">
         <v>130</v>
@@ -3800,34 +3811,34 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C5" t="s">
         <v>152</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" t="s">
         <v>256</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I5" t="s">
-        <v>257</v>
-      </c>
       <c r="J5" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="M5" t="s">
         <v>130</v>
@@ -3863,7 +3874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FBAD3F-B068-45FE-8F7E-81242A44B945}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -3907,94 +3918,94 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
@@ -4002,67 +4013,67 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" t="s">
         <v>296</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>297</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>298</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>299</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>300</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="N2" t="s">
+        <v>297</v>
+      </c>
+      <c r="O2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P2" t="s">
         <v>301</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="N2" t="s">
-        <v>298</v>
-      </c>
-      <c r="O2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>302</v>
       </c>
-      <c r="Q2" t="s">
-        <v>303</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="T2" t="s">
         <v>173</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="V2" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>146</v>
@@ -4071,10 +4082,10 @@
         <v>179</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>146</v>
@@ -4083,10 +4094,10 @@
         <v>184</v>
       </c>
       <c r="AC2" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>146</v>
@@ -4097,67 +4108,67 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H3" t="s">
+        <v>303</v>
+      </c>
+      <c r="I3" t="s">
         <v>304</v>
       </c>
-      <c r="I3" t="s">
-        <v>305</v>
-      </c>
       <c r="J3" t="s">
+        <v>298</v>
+      </c>
+      <c r="K3" t="s">
         <v>299</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>300</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="N3" t="s">
+        <v>297</v>
+      </c>
+      <c r="O3" t="s">
+        <v>298</v>
+      </c>
+      <c r="P3" t="s">
         <v>301</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="N3" t="s">
-        <v>298</v>
-      </c>
-      <c r="O3" t="s">
-        <v>299</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>302</v>
       </c>
-      <c r="Q3" t="s">
-        <v>303</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="T3" t="s">
         <v>179</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>146</v>
@@ -4166,22 +4177,22 @@
         <v>184</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>146</v>
       </c>
       <c r="AB3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AC3" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="AE3" s="2" t="s">
         <v>146</v>
@@ -4192,91 +4203,91 @@
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E4" t="s">
+        <v>295</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="H4" t="s">
         <v>296</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" t="s">
+        <v>298</v>
+      </c>
+      <c r="K4" t="s">
+        <v>299</v>
+      </c>
+      <c r="L4" t="s">
+        <v>300</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="N4" t="s">
         <v>297</v>
       </c>
-      <c r="I4" t="s">
-        <v>307</v>
-      </c>
-      <c r="J4" t="s">
-        <v>299</v>
-      </c>
-      <c r="K4" t="s">
-        <v>300</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
+        <v>298</v>
+      </c>
+      <c r="P4" t="s">
         <v>301</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="N4" t="s">
-        <v>298</v>
-      </c>
-      <c r="O4" t="s">
-        <v>299</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>302</v>
       </c>
-      <c r="Q4" t="s">
-        <v>303</v>
-      </c>
       <c r="R4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="T4" t="s">
         <v>184</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>146</v>
       </c>
       <c r="X4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>146</v>
       </c>
       <c r="AB4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AC4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="AE4" s="2" t="s">
         <v>146</v>
@@ -4287,79 +4298,79 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="H5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I5" t="s">
+        <v>308</v>
+      </c>
+      <c r="J5" t="s">
+        <v>298</v>
+      </c>
+      <c r="K5" t="s">
+        <v>299</v>
+      </c>
+      <c r="L5" t="s">
+        <v>300</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="N5" t="s">
+        <v>297</v>
+      </c>
+      <c r="O5" t="s">
+        <v>298</v>
+      </c>
+      <c r="P5" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>302</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="H5" t="s">
-        <v>304</v>
-      </c>
-      <c r="I5" t="s">
-        <v>309</v>
-      </c>
-      <c r="J5" t="s">
-        <v>299</v>
-      </c>
-      <c r="K5" t="s">
-        <v>300</v>
-      </c>
-      <c r="L5" t="s">
-        <v>301</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="N5" t="s">
-        <v>298</v>
-      </c>
-      <c r="O5" t="s">
-        <v>299</v>
-      </c>
-      <c r="P5" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>303</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>330</v>
-      </c>
       <c r="S5" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="T5" t="s">
+        <v>305</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="T5" t="s">
-        <v>306</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>334</v>
-      </c>
       <c r="V5" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>146</v>
       </c>
       <c r="X5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AA5" s="2" t="s">
         <v>146</v>
@@ -4368,10 +4379,10 @@
         <v>187</v>
       </c>
       <c r="AC5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD5" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="AE5" s="2" t="s">
         <v>146</v>
@@ -4388,7 +4399,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4422,76 +4433,76 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>368</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
@@ -4499,25 +4510,25 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C2" t="s">
         <v>370</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>371</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>372</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>373</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>374</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>375</v>
-      </c>
-      <c r="M2" t="s">
-        <v>376</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>146</v>
@@ -4526,25 +4537,25 @@
         <v>146</v>
       </c>
       <c r="P2" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q2" t="s">
         <v>377</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>377</v>
+      </c>
+      <c r="S2" t="s">
+        <v>377</v>
+      </c>
+      <c r="T2" t="s">
+        <v>377</v>
+      </c>
+      <c r="U2" t="s">
+        <v>377</v>
+      </c>
+      <c r="V2" t="s">
         <v>378</v>
-      </c>
-      <c r="R2" t="s">
-        <v>378</v>
-      </c>
-      <c r="S2" t="s">
-        <v>378</v>
-      </c>
-      <c r="T2" t="s">
-        <v>378</v>
-      </c>
-      <c r="U2" t="s">
-        <v>378</v>
-      </c>
-      <c r="V2" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
@@ -4552,25 +4563,25 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" t="s">
         <v>370</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>371</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>372</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>373</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>374</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>375</v>
-      </c>
-      <c r="M3" t="s">
-        <v>376</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>146</v>
@@ -4579,25 +4590,25 @@
         <v>146</v>
       </c>
       <c r="P3" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q3" t="s">
         <v>377</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
+        <v>377</v>
+      </c>
+      <c r="S3" t="s">
+        <v>377</v>
+      </c>
+      <c r="T3" t="s">
+        <v>377</v>
+      </c>
+      <c r="U3" t="s">
+        <v>377</v>
+      </c>
+      <c r="V3" t="s">
         <v>378</v>
-      </c>
-      <c r="R3" t="s">
-        <v>378</v>
-      </c>
-      <c r="S3" t="s">
-        <v>378</v>
-      </c>
-      <c r="T3" t="s">
-        <v>378</v>
-      </c>
-      <c r="U3" t="s">
-        <v>378</v>
-      </c>
-      <c r="V3" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
@@ -4605,25 +4616,25 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C4" t="s">
         <v>370</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>371</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>372</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>373</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>374</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>375</v>
-      </c>
-      <c r="M4" t="s">
-        <v>376</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>146</v>
@@ -4632,25 +4643,25 @@
         <v>146</v>
       </c>
       <c r="P4" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q4" t="s">
         <v>377</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
+        <v>377</v>
+      </c>
+      <c r="S4" t="s">
+        <v>377</v>
+      </c>
+      <c r="T4" t="s">
+        <v>377</v>
+      </c>
+      <c r="U4" t="s">
+        <v>377</v>
+      </c>
+      <c r="V4" t="s">
         <v>378</v>
-      </c>
-      <c r="R4" t="s">
-        <v>378</v>
-      </c>
-      <c r="S4" t="s">
-        <v>378</v>
-      </c>
-      <c r="T4" t="s">
-        <v>378</v>
-      </c>
-      <c r="U4" t="s">
-        <v>378</v>
-      </c>
-      <c r="V4" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
@@ -4658,25 +4669,25 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" t="s">
         <v>370</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>371</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>372</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>373</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>374</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>375</v>
-      </c>
-      <c r="M5" t="s">
-        <v>376</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>146</v>
@@ -4685,30 +4696,30 @@
         <v>146</v>
       </c>
       <c r="P5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q5" t="s">
         <v>377</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
+        <v>377</v>
+      </c>
+      <c r="S5" t="s">
+        <v>377</v>
+      </c>
+      <c r="T5" t="s">
+        <v>377</v>
+      </c>
+      <c r="U5" t="s">
+        <v>377</v>
+      </c>
+      <c r="V5" t="s">
         <v>378</v>
-      </c>
-      <c r="R5" t="s">
-        <v>378</v>
-      </c>
-      <c r="S5" t="s">
-        <v>378</v>
-      </c>
-      <c r="T5" t="s">
-        <v>378</v>
-      </c>
-      <c r="U5" t="s">
-        <v>378</v>
-      </c>
-      <c r="V5" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="P7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing add customer personal and company
</commit_message>
<xml_diff>
--- a/Data Files/LOS_Customer_TestData.xlsx
+++ b/Data Files/LOS_Customer_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\automation-taf-project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB667E-5B96-42D9-82AD-C086B3877C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F55EC9A-6842-4DE2-B930-7059E1A0B3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{BB2015A2-793C-446E-A619-E1E11BD5D040}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{BB2015A2-793C-446E-A619-E1E11BD5D040}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="FinancialData" sheetId="8" r:id="rId8"/>
     <sheet name="OtherAttribute" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="382">
   <si>
     <t>Username</t>
   </si>
@@ -200,15 +200,6 @@
     <t>12/12/2099</t>
   </si>
   <si>
-    <t>12/13/2099</t>
-  </si>
-  <si>
-    <t>12/14/2099</t>
-  </si>
-  <si>
-    <t>12/15/2099</t>
-  </si>
-  <si>
     <t>Salutation</t>
   </si>
   <si>
@@ -305,9 +296,6 @@
     <t>S2</t>
   </si>
   <si>
-    <t>Hindu</t>
-  </si>
-  <si>
     <t>S3</t>
   </si>
   <si>
@@ -1182,6 +1170,15 @@
   </si>
   <si>
     <t>Y/N</t>
+  </si>
+  <si>
+    <t>HINDU</t>
+  </si>
+  <si>
+    <t>RINIY</t>
+  </si>
+  <si>
+    <t>3203283107950006</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BA1AD0-7BFC-40B0-8219-A5C3FF6E1E54}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1765,13 +1762,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>380</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>381</v>
@@ -1780,19 +1777,19 @@
         <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>245</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1800,34 +1797,34 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1835,34 +1832,34 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1870,34 +1867,34 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>376</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>377</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>50</v>
+        <v>241</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -1907,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF85E20-BF5A-491B-8BD8-8C65920F3112}">
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1944,79 +1941,79 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
@@ -2024,28 +2021,25 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="O2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P2" t="s">
-        <v>86</v>
+        <v>379</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
@@ -2053,25 +2047,25 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" t="s">
         <v>87</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>88</v>
       </c>
-      <c r="O3" t="s">
-        <v>89</v>
-      </c>
-      <c r="P3" t="s">
-        <v>90</v>
-      </c>
       <c r="V3" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
@@ -2079,25 +2073,25 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>81</v>
+      </c>
+      <c r="N4" t="s">
+        <v>135</v>
       </c>
       <c r="O4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P4" t="s">
-        <v>92</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
@@ -2105,57 +2099,60 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" t="s">
         <v>135</v>
       </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M5" t="s">
-        <v>84</v>
-      </c>
-      <c r="N5" t="s">
-        <v>139</v>
-      </c>
       <c r="O5" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="P5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H8" t="s">
-        <v>140</v>
-      </c>
-      <c r="M8" t="s">
-        <v>140</v>
-      </c>
-      <c r="N8" t="s">
-        <v>141</v>
-      </c>
-      <c r="P8" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>382</v>
-      </c>
-      <c r="T8" t="s">
-        <v>382</v>
-      </c>
-      <c r="V8" t="s">
-        <v>140</v>
+        <v>83</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" t="s">
+        <v>136</v>
+      </c>
+      <c r="M7" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>378</v>
+      </c>
+      <c r="T7" t="s">
+        <v>378</v>
+      </c>
+      <c r="V7" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2167,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78014918-227A-4AF6-B3BB-0B6F0E9D6C98}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2197,64 +2194,64 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
@@ -2262,10 +2259,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>16</v>
@@ -2274,49 +2271,49 @@
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="O2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="P2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="T2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -2324,61 +2321,61 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I3" t="s">
         <v>39</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="O3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="P3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="T3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="U3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -2386,61 +2383,61 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I4" t="s">
         <v>39</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="N4" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="O4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="T4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="U4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
@@ -2448,10 +2445,10 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -2460,49 +2457,49 @@
         <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I5" t="s">
         <v>39</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="N5" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="O5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="P5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="T5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -2510,61 +2507,61 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I6" t="s">
         <v>39</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="O6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="P6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="T6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="U6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -2572,61 +2569,61 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="O7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="T7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="U7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -2634,10 +2631,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
@@ -2646,49 +2643,49 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="O8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="P8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="T8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
@@ -2696,61 +2693,61 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I9" t="s">
         <v>39</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="O9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="P9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="T9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="U9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -2758,61 +2755,61 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I10" t="s">
         <v>39</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O10" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="T10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="U10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -2820,10 +2817,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>16</v>
@@ -2832,49 +2829,49 @@
         <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I11" t="s">
         <v>39</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="O11" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="P11" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="T11" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
@@ -2882,61 +2879,61 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I12" t="s">
         <v>39</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O12" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="P12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="T12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="U12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
@@ -2944,66 +2941,66 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I13" t="s">
         <v>39</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="O13" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="S13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="T13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="U13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="J14" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -3041,7 +3038,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>21</v>
@@ -3068,7 +3065,7 @@
         <v>28</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -3085,7 +3082,7 @@
         <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>54</v>
@@ -3100,13 +3097,13 @@
         <v>53</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K2" t="s">
         <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -3144,7 +3141,7 @@
         <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -3182,7 +3179,7 @@
         <v>47</v>
       </c>
       <c r="L4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -3220,7 +3217,7 @@
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3233,8 +3230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE94967-9968-4388-93D5-8EE5D91AC311}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3267,67 +3264,67 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="P1" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
@@ -3335,55 +3332,55 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>168</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L2" t="s">
         <v>169</v>
       </c>
-      <c r="F2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="O2" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="H2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="P2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="R2" t="s">
         <v>171</v>
-      </c>
-      <c r="J2" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="L2" t="s">
-        <v>173</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="O2" t="s">
-        <v>174</v>
-      </c>
-      <c r="P2" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="R2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
@@ -3391,55 +3388,55 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="H3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="O3" t="s">
+        <v>170</v>
+      </c>
+      <c r="P3" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="O3" t="s">
-        <v>174</v>
-      </c>
-      <c r="P3" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="R3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -3447,55 +3444,55 @@
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J4" t="s">
+        <v>179</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L4" t="s">
         <v>180</v>
       </c>
-      <c r="E4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" t="s">
-        <v>181</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="H4" t="s">
-        <v>167</v>
-      </c>
-      <c r="I4" t="s">
-        <v>182</v>
-      </c>
-      <c r="J4" t="s">
-        <v>183</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="L4" t="s">
-        <v>184</v>
-      </c>
       <c r="M4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="O4" t="s">
+        <v>170</v>
+      </c>
+      <c r="P4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="O4" t="s">
-        <v>174</v>
-      </c>
-      <c r="P4" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="R4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
@@ -3503,60 +3500,60 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="J5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="H5" t="s">
-        <v>167</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
+        <v>183</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="O5" t="s">
+        <v>170</v>
+      </c>
+      <c r="P5" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="R5" t="s">
         <v>171</v>
-      </c>
-      <c r="J5" t="s">
-        <v>183</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L5" t="s">
-        <v>187</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="O5" t="s">
-        <v>174</v>
-      </c>
-      <c r="P5" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="R5" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -3575,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4BC9DE-FDC7-4630-99DC-CABF00157D5F}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3596,55 +3593,55 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="R1" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -3652,52 +3649,52 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="I2" t="s">
-        <v>256</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>264</v>
+        <v>141</v>
       </c>
       <c r="M2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="N2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O2" t="s">
         <v>39</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -3705,52 +3702,52 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="M3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O3" t="s">
         <v>39</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -3758,52 +3755,52 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="I4" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C4" t="s">
+      <c r="L4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="I4" t="s">
-        <v>256</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>264</v>
-      </c>
       <c r="M4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="N4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O4" t="s">
         <v>39</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -3811,60 +3808,60 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>248</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>263</v>
+        <v>17</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="M5" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="N5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O5" t="s">
         <v>39</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{7B972C15-22F0-44F4-8D58-4EA9FFBBE6BE}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{883E24D6-7BE5-44B6-9A8E-AF07A4B9BAA1}"/>
-    <hyperlink ref="G3:H5" r:id="rId3" display="testtt@gmail.com" xr:uid="{A3CDEB75-8354-41C0-BA2F-4173F4898DF2}"/>
+    <hyperlink ref="G2:H4" r:id="rId1" display="testtt@gmail.com" xr:uid="{A3CDEB75-8354-41C0-BA2F-4173F4898DF2}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{1619406B-6E08-4633-9C23-B191B51E1F0C}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{195B6D60-4690-4D26-B9E6-EF2B74DF05A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3874,8 +3871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92FBAD3F-B068-45FE-8F7E-81242A44B945}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3918,94 +3915,94 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
@@ -4013,94 +4010,94 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K2" t="s">
         <v>295</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="L2" t="s">
+        <v>296</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N2" t="s">
+        <v>293</v>
+      </c>
+      <c r="O2" t="s">
+        <v>294</v>
+      </c>
+      <c r="P2" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>298</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H2" t="s">
-        <v>296</v>
-      </c>
-      <c r="I2" t="s">
-        <v>297</v>
-      </c>
-      <c r="J2" t="s">
-        <v>298</v>
-      </c>
-      <c r="K2" t="s">
-        <v>299</v>
-      </c>
-      <c r="L2" t="s">
-        <v>300</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="N2" t="s">
-        <v>297</v>
-      </c>
-      <c r="O2" t="s">
-        <v>298</v>
-      </c>
-      <c r="P2" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>302</v>
-      </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="T2" t="s">
+        <v>169</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="T2" t="s">
-        <v>173</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>333</v>
-      </c>
       <c r="V2" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="X2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AB2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -4108,94 +4105,94 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H3" t="s">
+        <v>299</v>
+      </c>
+      <c r="I3" t="s">
+        <v>300</v>
+      </c>
+      <c r="J3" t="s">
+        <v>294</v>
+      </c>
+      <c r="K3" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="L3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N3" t="s">
+        <v>293</v>
+      </c>
+      <c r="O3" t="s">
+        <v>294</v>
+      </c>
+      <c r="P3" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>298</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H3" t="s">
-        <v>303</v>
-      </c>
-      <c r="I3" t="s">
-        <v>304</v>
-      </c>
-      <c r="J3" t="s">
-        <v>298</v>
-      </c>
-      <c r="K3" t="s">
-        <v>299</v>
-      </c>
-      <c r="L3" t="s">
-        <v>300</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="N3" t="s">
-        <v>297</v>
-      </c>
-      <c r="O3" t="s">
-        <v>298</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="S3" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="T3" t="s">
+        <v>175</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="X3" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB3" t="s">
         <v>301</v>
       </c>
-      <c r="Q3" t="s">
-        <v>302</v>
-      </c>
-      <c r="R3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="T3" t="s">
-        <v>179</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="X3" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>305</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>334</v>
-      </c>
       <c r="AE3" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
@@ -4203,94 +4200,94 @@
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="H4" t="s">
+        <v>292</v>
+      </c>
+      <c r="I4" t="s">
+        <v>302</v>
+      </c>
+      <c r="J4" t="s">
+        <v>294</v>
+      </c>
+      <c r="K4" t="s">
         <v>295</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="L4" t="s">
+        <v>296</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N4" t="s">
+        <v>293</v>
+      </c>
+      <c r="O4" t="s">
+        <v>294</v>
+      </c>
+      <c r="P4" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>298</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="H4" t="s">
-        <v>296</v>
-      </c>
-      <c r="I4" t="s">
-        <v>306</v>
-      </c>
-      <c r="J4" t="s">
-        <v>298</v>
-      </c>
-      <c r="K4" t="s">
-        <v>299</v>
-      </c>
-      <c r="L4" t="s">
-        <v>300</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="N4" t="s">
-        <v>297</v>
-      </c>
-      <c r="O4" t="s">
-        <v>298</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="S4" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="T4" t="s">
+        <v>180</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="X4" t="s">
         <v>301</v>
       </c>
-      <c r="Q4" t="s">
-        <v>302</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="S4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z4" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="T4" t="s">
-        <v>184</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="X4" t="s">
-        <v>305</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="AA4" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AB4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
@@ -4298,94 +4295,94 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>291</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H5" t="s">
+        <v>299</v>
+      </c>
+      <c r="I5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>294</v>
+      </c>
+      <c r="K5" t="s">
         <v>295</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="L5" t="s">
+        <v>296</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N5" t="s">
+        <v>293</v>
+      </c>
+      <c r="O5" t="s">
+        <v>294</v>
+      </c>
+      <c r="P5" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>298</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="H5" t="s">
+      <c r="T5" t="s">
+        <v>301</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="X5" t="s">
         <v>303</v>
       </c>
-      <c r="I5" t="s">
-        <v>308</v>
-      </c>
-      <c r="J5" t="s">
-        <v>298</v>
-      </c>
-      <c r="K5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L5" t="s">
-        <v>300</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="N5" t="s">
-        <v>297</v>
-      </c>
-      <c r="O5" t="s">
-        <v>298</v>
-      </c>
-      <c r="P5" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>302</v>
-      </c>
-      <c r="R5" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="T5" t="s">
-        <v>305</v>
-      </c>
-      <c r="U5" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="V5" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="X5" t="s">
-        <v>307</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>337</v>
-      </c>
       <c r="AA5" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AB5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4433,76 +4430,76 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
@@ -4510,52 +4507,52 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H2" t="s">
         <v>369</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
         <v>370</v>
       </c>
-      <c r="D2" t="s">
+      <c r="M2" t="s">
         <v>371</v>
       </c>
-      <c r="E2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P2" t="s">
         <v>372</v>
       </c>
-      <c r="H2" t="s">
+      <c r="Q2" t="s">
         <v>373</v>
       </c>
-      <c r="I2" t="s">
+      <c r="R2" t="s">
+        <v>373</v>
+      </c>
+      <c r="S2" t="s">
+        <v>373</v>
+      </c>
+      <c r="T2" t="s">
+        <v>373</v>
+      </c>
+      <c r="U2" t="s">
+        <v>373</v>
+      </c>
+      <c r="V2" t="s">
         <v>374</v>
-      </c>
-      <c r="M2" t="s">
-        <v>375</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="P2" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>377</v>
-      </c>
-      <c r="R2" t="s">
-        <v>377</v>
-      </c>
-      <c r="S2" t="s">
-        <v>377</v>
-      </c>
-      <c r="T2" t="s">
-        <v>377</v>
-      </c>
-      <c r="U2" t="s">
-        <v>377</v>
-      </c>
-      <c r="V2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
@@ -4563,52 +4560,52 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" t="s">
+        <v>368</v>
+      </c>
+      <c r="H3" t="s">
         <v>369</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
         <v>370</v>
       </c>
-      <c r="D3" t="s">
+      <c r="M3" t="s">
         <v>371</v>
       </c>
-      <c r="E3" t="s">
+      <c r="N3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P3" t="s">
         <v>372</v>
       </c>
-      <c r="H3" t="s">
+      <c r="Q3" t="s">
         <v>373</v>
       </c>
-      <c r="I3" t="s">
+      <c r="R3" t="s">
+        <v>373</v>
+      </c>
+      <c r="S3" t="s">
+        <v>373</v>
+      </c>
+      <c r="T3" t="s">
+        <v>373</v>
+      </c>
+      <c r="U3" t="s">
+        <v>373</v>
+      </c>
+      <c r="V3" t="s">
         <v>374</v>
-      </c>
-      <c r="M3" t="s">
-        <v>375</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="P3" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>377</v>
-      </c>
-      <c r="R3" t="s">
-        <v>377</v>
-      </c>
-      <c r="S3" t="s">
-        <v>377</v>
-      </c>
-      <c r="T3" t="s">
-        <v>377</v>
-      </c>
-      <c r="U3" t="s">
-        <v>377</v>
-      </c>
-      <c r="V3" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
@@ -4616,52 +4613,52 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E4" t="s">
+        <v>368</v>
+      </c>
+      <c r="H4" t="s">
         <v>369</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I4" t="s">
         <v>370</v>
       </c>
-      <c r="D4" t="s">
+      <c r="M4" t="s">
         <v>371</v>
       </c>
-      <c r="E4" t="s">
+      <c r="N4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P4" t="s">
         <v>372</v>
       </c>
-      <c r="H4" t="s">
+      <c r="Q4" t="s">
         <v>373</v>
       </c>
-      <c r="I4" t="s">
+      <c r="R4" t="s">
+        <v>373</v>
+      </c>
+      <c r="S4" t="s">
+        <v>373</v>
+      </c>
+      <c r="T4" t="s">
+        <v>373</v>
+      </c>
+      <c r="U4" t="s">
+        <v>373</v>
+      </c>
+      <c r="V4" t="s">
         <v>374</v>
-      </c>
-      <c r="M4" t="s">
-        <v>375</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="P4" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>377</v>
-      </c>
-      <c r="R4" t="s">
-        <v>377</v>
-      </c>
-      <c r="S4" t="s">
-        <v>377</v>
-      </c>
-      <c r="T4" t="s">
-        <v>377</v>
-      </c>
-      <c r="U4" t="s">
-        <v>377</v>
-      </c>
-      <c r="V4" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
@@ -4669,57 +4666,57 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E5" t="s">
+        <v>368</v>
+      </c>
+      <c r="H5" t="s">
         <v>369</v>
       </c>
-      <c r="C5" t="s">
+      <c r="I5" t="s">
         <v>370</v>
       </c>
-      <c r="D5" t="s">
+      <c r="M5" t="s">
         <v>371</v>
       </c>
-      <c r="E5" t="s">
+      <c r="N5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P5" t="s">
         <v>372</v>
       </c>
-      <c r="H5" t="s">
+      <c r="Q5" t="s">
         <v>373</v>
       </c>
-      <c r="I5" t="s">
+      <c r="R5" t="s">
+        <v>373</v>
+      </c>
+      <c r="S5" t="s">
+        <v>373</v>
+      </c>
+      <c r="T5" t="s">
+        <v>373</v>
+      </c>
+      <c r="U5" t="s">
+        <v>373</v>
+      </c>
+      <c r="V5" t="s">
         <v>374</v>
-      </c>
-      <c r="M5" t="s">
-        <v>375</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="P5" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>377</v>
-      </c>
-      <c r="R5" t="s">
-        <v>377</v>
-      </c>
-      <c r="S5" t="s">
-        <v>377</v>
-      </c>
-      <c r="T5" t="s">
-        <v>377</v>
-      </c>
-      <c r="U5" t="s">
-        <v>377</v>
-      </c>
-      <c r="V5" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="P7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing ss and scripting nap
</commit_message>
<xml_diff>
--- a/Data Files/LOS_Customer_TestData.xlsx
+++ b/Data Files/LOS_Customer_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\automation-taf-project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E732B5F-0764-4BE2-A771-3EA7A53669D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20403354-A545-489E-8CA3-FBA3213FB359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BB2015A2-793C-446E-A619-E1E11BD5D040}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{BB2015A2-793C-446E-A619-E1E11BD5D040}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -1175,10 +1175,10 @@
     <t>HINDU</t>
   </si>
   <si>
-    <t>RINIF</t>
-  </si>
-  <si>
-    <t>3203283107950013</t>
+    <t>VANILA</t>
+  </si>
+  <si>
+    <t>3203283107950021</t>
   </si>
 </sst>
 </file>
@@ -1704,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BA1AD0-7BFC-40B0-8219-A5C3FF6E1E54}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" activeCellId="1" sqref="C10 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1906,7 +1906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF85E20-BF5A-491B-8BD8-8C65920F3112}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>